<commit_message>
ggplot, gt, fs, DataTest add tests for readxl, tidy_*
</commit_message>
<xml_diff>
--- a/inst/extdata/ExcelData_Example.xlsx
+++ b/inst/extdata/ExcelData_Example.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GC Projects\My Tools\onepunch\quantre\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCB9BD7-5807-4CFB-9CF4-393CAABFE9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F561E-C9E9-4EC5-B924-044B00008844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{02E692AA-A256-4D1B-9D90-D7FB403A1E1F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{02E692AA-A256-4D1B-9D90-D7FB403A1E1F}"/>
   </bookViews>
   <sheets>
     <sheet name="BlockData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DataType" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="DataFrame">DataType!$B$2:$E$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Band</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +72,62 @@
   </si>
   <si>
     <t>Class2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nationality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>China</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -209,7 +268,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -235,6 +294,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE905F7-698C-4C48-B95C-6E71EA469414}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -837,16 +899,16 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>0</v>
@@ -1016,14 +1078,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E8CF5D-8C4C-4FFB-AE05-1337312A2B77}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3.1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>43466</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3.14</v>
+      </c>
+      <c r="E4" s="9">
+        <v>44196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3.141</v>
+      </c>
+      <c r="E5" s="9">
+        <v>44377</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>